<commit_message>
Separate Columns: PO Number, WO Number, Job Number. Remove From Pressure Zone/To Pressure Zone. Add new column: Heat Number (after MFR Model Number). In Station details screen, Pressure Document Information should have record identifier column. Disable/Enable OD, WT, Grade, Rating and Seam drop downs based on Rated/Non-Rated feature types. Two OD dropdowns: nominal for feature type rated , actual for non-rated.
</commit_message>
<xml_diff>
--- a/PLF Dev Sprint Estimates.xlsx
+++ b/PLF Dev Sprint Estimates.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Surendra\PFL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9932B55A-F9E1-418D-A882-AEEFCDC16E58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE733CB-DCA1-4D12-92B7-B7C2E5CE4EB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="4740" xr2:uid="{D9AB06D8-2FE9-40A8-A439-2F99B4ECD2CD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="4740" activeTab="1" xr2:uid="{D9AB06D8-2FE9-40A8-A439-2F99B4ECD2CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="DataModel Updates" sheetId="3" r:id="rId2"/>
-    <sheet name="ANSI rating" sheetId="2" r:id="rId3"/>
-    <sheet name="Grades" sheetId="4" r:id="rId4"/>
-    <sheet name="SeamTypes" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId4"/>
+    <sheet name="ANSI rating" sheetId="2" r:id="rId5"/>
+    <sheet name="Grades" sheetId="4" r:id="rId6"/>
+    <sheet name="SeamTypes" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="228">
   <si>
     <t>Feature</t>
   </si>
@@ -370,9 +372,6 @@
   </si>
   <si>
     <t>PressureRating</t>
-  </si>
-  <si>
-    <t>Table</t>
   </si>
   <si>
     <t>Update</t>
@@ -633,33 +632,6 @@
     <t>Rated/Non-Rated</t>
   </si>
   <si>
-    <t>created_Date</t>
-  </si>
-  <si>
-    <t>code_lookup_name</t>
-  </si>
-  <si>
-    <t>old_value</t>
-  </si>
-  <si>
-    <t>new_value</t>
-  </si>
-  <si>
-    <t>created_user</t>
-  </si>
-  <si>
-    <t>update_user</t>
-  </si>
-  <si>
-    <t>updated_date</t>
-  </si>
-  <si>
-    <t>action</t>
-  </si>
-  <si>
-    <t>logid</t>
-  </si>
-  <si>
     <t>Valvesectionfeatures column</t>
   </si>
   <si>
@@ -697,12 +669,244 @@
   </si>
   <si>
     <t>PTMedium in PressureTestRecords table</t>
+  </si>
+  <si>
+    <t>CodeLookUpAudit</t>
+  </si>
+  <si>
+    <t>Table/Stored procedure</t>
+  </si>
+  <si>
+    <t>spInsert_dbo_CodeLookUpAudit</t>
+  </si>
+  <si>
+    <t>ValveSectionFeatures</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Need to delete JobWOPO, JobWOPOUnknown, FromSeries and ToSeries columns</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Added new column: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PTRIDName</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Created new table</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> CodeLookUpAudit</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Added new columns: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> PONumber, POUnknown, WONumber, WOUnknown, JobNumber, JobUnknown</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HeatNumber</t>
+    </r>
+  </si>
+  <si>
+    <t>Concatenate PTR record identifier and file name</t>
+  </si>
+  <si>
+    <t>Two OD dropdowns: nominal for feature type rated , actual for non-rated</t>
+  </si>
+  <si>
+    <t>Disable/Enable OD, WT, Grade, Rating and Seam drop downs based on Rated/Non-Rated feature types</t>
+  </si>
+  <si>
+    <t>OutsideDiameters</t>
+  </si>
+  <si>
+    <t>PressureTestRecords</t>
+  </si>
+  <si>
+    <r>
+      <t>Created new stored procedure</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> spInsert_dbo_CodeLookUpAudit</t>
+    </r>
+  </si>
+  <si>
+    <t>OD 1 (Non-Rated)</t>
+  </si>
+  <si>
+    <t>Nominal OD in decimal (Rated)</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Added new column: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LengthLookup</t>
+    </r>
+  </si>
+  <si>
+    <t>Outside Diameter</t>
+  </si>
+  <si>
+    <t>90 Degree_1R (Short Radius)</t>
+  </si>
+  <si>
+    <t>90 Degree_1.5R (LR, Long Radius)</t>
+  </si>
+  <si>
+    <t>90 Degree_3R</t>
+  </si>
+  <si>
+    <t>90 Degree_Unknown Radius</t>
+  </si>
+  <si>
+    <t>45 Degree_1R (Short Radius)</t>
+  </si>
+  <si>
+    <t>45 Degree_1.5R (LR, Long Radius)</t>
+  </si>
+  <si>
+    <t>45 Degree_3R</t>
+  </si>
+  <si>
+    <t>45 Degree_Unknown Radius</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  </t>
+  </si>
+  <si>
+    <t>, Degree90_1_5R =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, Degree90_3R = </t>
+  </si>
+  <si>
+    <t>, Degree90_Unknown =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, Degree45_Unknown = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">, Degree45_3R = </t>
+  </si>
+  <si>
+    <t>, Degree45_1_5R =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, Degree45_1R = </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> where [OutsideDiameterItem] =  </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Added new columns </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NominalDiameterItem</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and populated values</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -755,13 +959,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -819,53 +1023,80 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1181,19 +1412,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E82D264-ABBD-4D6C-A133-C27B2E8FBD86}">
-  <dimension ref="A1:T32"/>
+  <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12:I12"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="5.1171875" customWidth="1"/>
-    <col min="2" max="2" width="46.5859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="86.234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5859375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.41015625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.1171875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.05859375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.05859375" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.64453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.46875" customWidth="1"/>
     <col min="9" max="9" width="32.703125" bestFit="1" customWidth="1"/>
@@ -1216,266 +1448,266 @@
         <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="I1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1" s="19"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A2" s="14">
+        <v>10</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A3" s="5"/>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8">
+        <v>6</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A4" s="5"/>
+      <c r="B4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8">
+        <v>6</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A5" s="5"/>
+      <c r="B5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8">
+        <v>6</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A6" s="5"/>
+      <c r="B6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8">
+        <v>6</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A7" s="5"/>
+      <c r="B7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8">
+        <v>6</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A8" s="5"/>
+      <c r="B8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="8">
+        <v>6</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A9" s="5"/>
+      <c r="B9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="8">
+        <v>6</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A10" s="5"/>
+      <c r="B10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="8">
+        <v>6</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A11" s="5"/>
+      <c r="B11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="8">
+        <v>6</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A12" s="5"/>
+      <c r="B12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="8">
+        <v>6</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A2" s="18">
-        <v>10</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A3" s="6"/>
-      <c r="B3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="9">
-        <v>6</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="16" t="s">
+      <c r="I12" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="I3" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A4" s="6"/>
-      <c r="B4" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="9">
-        <v>6</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A5" s="6"/>
-      <c r="B5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="9">
-        <v>6</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="I5" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A6" s="6"/>
-      <c r="B6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="9">
-        <v>6</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A7" s="6"/>
-      <c r="B7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="9">
-        <v>6</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="I7" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A8" s="6"/>
-      <c r="B8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="9">
-        <v>6</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A9" s="6"/>
-      <c r="B9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="9">
-        <v>6</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A10" s="6"/>
-      <c r="B10" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="9">
-        <v>6</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="I10" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A11" s="6"/>
-      <c r="B11" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="9">
-        <v>6</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="I11" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A12" s="6"/>
-      <c r="B12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="9">
-        <v>6</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="I12" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A13" s="3">
@@ -1487,11 +1719,11 @@
       <c r="C13" s="3">
         <v>8</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A14" s="3">
@@ -1505,166 +1737,142 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A15" s="3">
+      <c r="A15" s="5">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
+      <c r="C15" s="5"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="5">
         <v>24</v>
       </c>
-      <c r="G16" t="s">
-        <v>184</v>
-      </c>
-      <c r="H16" t="s">
-        <v>177</v>
-      </c>
-      <c r="I16" t="s">
-        <v>178</v>
-      </c>
-      <c r="J16" t="s">
-        <v>179</v>
-      </c>
-      <c r="K16" t="s">
-        <v>183</v>
-      </c>
-      <c r="L16" t="s">
-        <v>180</v>
-      </c>
-      <c r="M16" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="N16" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="O16" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="13"/>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="5">
         <v>24</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="5">
         <v>24</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A19" s="6">
+      <c r="A19" s="5">
         <v>14</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>8</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A20" s="6">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>8</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A21" s="3">
@@ -1676,252 +1884,341 @@
       <c r="C21" s="3">
         <v>16</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A22" s="11">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="5">
+        <v>12</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A23" s="11">
-        <v>22</v>
-      </c>
-      <c r="B23" s="11" t="s">
+      <c r="C23" s="5">
+        <v>2</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A24" s="11">
-        <v>23</v>
-      </c>
-      <c r="B24" s="11" t="s">
+      <c r="C24" s="5">
+        <v>2</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+    </row>
+    <row r="25" spans="1:20" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13"/>
-      <c r="T24" s="13"/>
-    </row>
-    <row r="25" spans="1:20" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A25" s="11">
-        <v>24</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13"/>
+      <c r="C25" s="5">
+        <v>4</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4" t="s">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="C26" s="5">
+        <v>4</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="C27" s="5">
+        <v>12</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C28" s="5">
         <v>16</v>
       </c>
-      <c r="C26" s="3">
-        <f>SUM(C3:C21)</f>
-        <v>204</v>
-      </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="13"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="B27" s="1"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="B28" s="1"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="B29" s="1"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="13"/>
-      <c r="R29" s="13"/>
-      <c r="S29" s="13"/>
-      <c r="T29" s="13"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="3">
+        <f>SUM(C2:C28)</f>
+        <v>256</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="B30" s="1"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="13"/>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13"/>
-      <c r="T30" s="13"/>
-    </row>
-    <row r="31" spans="1:20" ht="57.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="13"/>
-      <c r="R31" s="13"/>
-      <c r="S31" s="13"/>
-      <c r="T31" s="13"/>
+      <c r="B30" s="3"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.5">
+      <c r="B31" s="1"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.5">
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
+      <c r="B32" s="1"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="9"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.5">
+      <c r="B33" s="1"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="9"/>
+      <c r="S33" s="9"/>
+      <c r="T33" s="9"/>
+    </row>
+    <row r="34" spans="2:20" ht="57.7" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
+      <c r="R34" s="9"/>
+      <c r="S34" s="9"/>
+      <c r="T34" s="9"/>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.5">
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
     </row>
   </sheetData>
   <sortState ref="B3:E12">
@@ -1934,48 +2231,108 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33E479CB-9735-45BE-8193-E9A7B1E37F73}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="10.29296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.17578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.41015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="98.17578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.87890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A1" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A2" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
+      <c r="B2" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="B2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="B3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A4" t="s">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A4" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" s="33" t="s">
         <v>173</v>
       </c>
-      <c r="B4" t="s">
-        <v>174</v>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A5" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A6" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A7" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1985,6 +2342,2045 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F4F532B-3A36-4DD0-B7D4-8571B4AB4692}">
+  <dimension ref="A1:W27"/>
+  <sheetViews>
+    <sheetView topLeftCell="S1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="6.52734375" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.703125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="7.76171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.46875" customWidth="1"/>
+    <col min="5" max="5" width="8.9375" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
+    <col min="13" max="13" width="36.87890625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.9375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.9375" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.05859375" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.703125" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.703125" style="4" customWidth="1"/>
+    <col min="19" max="19" width="15.29296875" style="4" customWidth="1"/>
+    <col min="20" max="20" width="20.05859375" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.05859375" style="4" customWidth="1"/>
+    <col min="22" max="22" width="32.234375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="174.52734375" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="71.7" x14ac:dyDescent="0.5">
+      <c r="A1" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+    </row>
+    <row r="2" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A2" s="24">
+        <v>0.84</v>
+      </c>
+      <c r="B2" s="27">
+        <v>6.5449791666666701E-2</v>
+      </c>
+      <c r="C2" s="27">
+        <v>9.8174687499999996E-2</v>
+      </c>
+      <c r="D2" s="27">
+        <v>0.19634937499999999</v>
+      </c>
+      <c r="E2" s="27">
+        <v>6.544979166666666E-2</v>
+      </c>
+      <c r="F2" s="27">
+        <v>3.272489583333333E-2</v>
+      </c>
+      <c r="G2" s="27">
+        <v>4.9087343749999998E-2</v>
+      </c>
+      <c r="H2" s="27">
+        <v>9.8174687499999996E-2</v>
+      </c>
+      <c r="I2" s="27">
+        <v>3.272489583333333E-2</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V2" t="s">
+        <v>226</v>
+      </c>
+      <c r="W2" s="29" t="str">
+        <f>CONCATENATE(M2,TEXT(B2,"0.00"),N2,TEXT(C2,"0.00"),O2,TEXT(D2,"0.00"),P2,TEXT(E2,"0.00"),Q2,TEXT(F2,"0.00"),R2,TEXT(G2,"0.00"),S2,TEXT(H2,"0.00"),T2,TEXT(I2,"0.00"),V2,A2, ";")</f>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  0.07, Degree90_1_5R =0.10, Degree90_3R = 0.20, Degree90_Unknown =0.07, Degree45_1R = 0.03, Degree45_1_5R =0.05, Degree45_3R = 0.10, Degree45_Unknown = 0.03 where [OutsideDiameterItem] =  0.84;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A3" s="24">
+        <v>1.05</v>
+      </c>
+      <c r="B3" s="27">
+        <v>9.8174687499999982E-2</v>
+      </c>
+      <c r="C3" s="27">
+        <v>0.14726203124999998</v>
+      </c>
+      <c r="D3" s="27">
+        <v>0.29452406249999996</v>
+      </c>
+      <c r="E3" s="27">
+        <v>9.8174687499999982E-2</v>
+      </c>
+      <c r="F3" s="27">
+        <v>4.9087343749999991E-2</v>
+      </c>
+      <c r="G3" s="27">
+        <v>7.363101562499999E-2</v>
+      </c>
+      <c r="H3" s="27">
+        <v>0.14726203124999998</v>
+      </c>
+      <c r="I3" s="27">
+        <v>4.9087343749999991E-2</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V3" t="s">
+        <v>226</v>
+      </c>
+      <c r="W3" s="29" t="str">
+        <f t="shared" ref="W3:W27" si="0">CONCATENATE(M3,TEXT(B3,"0.00"),N3,TEXT(C3,"0.00"),O3,TEXT(D3,"0.00"),P3,TEXT(E3,"0.00"),Q3,TEXT(F3,"0.00"),R3,TEXT(G3,"0.00"),S3,TEXT(H3,"0.00"),T3,TEXT(I3,"0.00"),V3,A3, ";")</f>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  0.10, Degree90_1_5R =0.15, Degree90_3R = 0.29, Degree90_Unknown =0.10, Degree45_1R = 0.05, Degree45_1_5R =0.07, Degree45_3R = 0.15, Degree45_Unknown = 0.05 where [OutsideDiameterItem] =  1.05;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A4" s="24">
+        <v>1.3149999999999999</v>
+      </c>
+      <c r="B4" s="27">
+        <v>0.13089958333333332</v>
+      </c>
+      <c r="C4" s="27">
+        <v>0.19634937499999999</v>
+      </c>
+      <c r="D4" s="27">
+        <v>0.39269874999999999</v>
+      </c>
+      <c r="E4" s="27">
+        <v>0.13089958333333332</v>
+      </c>
+      <c r="F4" s="27">
+        <v>6.544979166666666E-2</v>
+      </c>
+      <c r="G4" s="27">
+        <v>9.8174687499999996E-2</v>
+      </c>
+      <c r="H4" s="27">
+        <v>0.19634937499999999</v>
+      </c>
+      <c r="I4" s="27">
+        <v>6.544979166666666E-2</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K4" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="L4" s="28"/>
+      <c r="M4" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V4" t="s">
+        <v>226</v>
+      </c>
+      <c r="W4" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  0.13, Degree90_1_5R =0.20, Degree90_3R = 0.39, Degree90_Unknown =0.13, Degree45_1R = 0.07, Degree45_1_5R =0.10, Degree45_3R = 0.20, Degree45_Unknown = 0.07 where [OutsideDiameterItem] =  1.315;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A5" s="24">
+        <v>1.66</v>
+      </c>
+      <c r="B5" s="27">
+        <v>0.16362447916666667</v>
+      </c>
+      <c r="C5" s="27">
+        <v>0.24543671875</v>
+      </c>
+      <c r="D5" s="27">
+        <v>0.49087343750000001</v>
+      </c>
+      <c r="E5" s="27">
+        <v>0.16362447916666667</v>
+      </c>
+      <c r="F5" s="27">
+        <v>8.1812239583333335E-2</v>
+      </c>
+      <c r="G5" s="27">
+        <v>0.122718359375</v>
+      </c>
+      <c r="H5" s="27">
+        <v>0.24543671875</v>
+      </c>
+      <c r="I5" s="27">
+        <v>8.1812239583333335E-2</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V5" t="s">
+        <v>226</v>
+      </c>
+      <c r="W5" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  0.16, Degree90_1_5R =0.25, Degree90_3R = 0.49, Degree90_Unknown =0.16, Degree45_1R = 0.08, Degree45_1_5R =0.12, Degree45_3R = 0.25, Degree45_Unknown = 0.08 where [OutsideDiameterItem] =  1.66;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A6" s="24">
+        <v>1.9</v>
+      </c>
+      <c r="B6" s="27">
+        <v>0.19634937499999996</v>
+      </c>
+      <c r="C6" s="27">
+        <v>0.29452406249999996</v>
+      </c>
+      <c r="D6" s="27">
+        <v>0.58904812499999992</v>
+      </c>
+      <c r="E6" s="27">
+        <v>0.19634937499999996</v>
+      </c>
+      <c r="F6" s="27">
+        <v>9.8174687499999982E-2</v>
+      </c>
+      <c r="G6" s="27">
+        <v>0.14726203124999998</v>
+      </c>
+      <c r="H6" s="27">
+        <v>0.29452406249999996</v>
+      </c>
+      <c r="I6" s="27">
+        <v>9.8174687499999982E-2</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V6" t="s">
+        <v>226</v>
+      </c>
+      <c r="W6" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  0.20, Degree90_1_5R =0.29, Degree90_3R = 0.59, Degree90_Unknown =0.20, Degree45_1R = 0.10, Degree45_1_5R =0.15, Degree45_3R = 0.29, Degree45_Unknown = 0.10 where [OutsideDiameterItem] =  1.9;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A7" s="24">
+        <v>2.375</v>
+      </c>
+      <c r="B7" s="27">
+        <v>0.26179916666666664</v>
+      </c>
+      <c r="C7" s="27">
+        <v>0.39269874999999999</v>
+      </c>
+      <c r="D7" s="27">
+        <v>0.78539749999999997</v>
+      </c>
+      <c r="E7" s="27">
+        <v>0.26179916666666664</v>
+      </c>
+      <c r="F7" s="27">
+        <v>0.13089958333333332</v>
+      </c>
+      <c r="G7" s="27">
+        <v>0.19634937499999999</v>
+      </c>
+      <c r="H7" s="27">
+        <v>0.39269874999999999</v>
+      </c>
+      <c r="I7" s="27">
+        <v>0.13089958333333332</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V7" t="s">
+        <v>226</v>
+      </c>
+      <c r="W7" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  0.26, Degree90_1_5R =0.39, Degree90_3R = 0.79, Degree90_Unknown =0.26, Degree45_1R = 0.13, Degree45_1_5R =0.20, Degree45_3R = 0.39, Degree45_Unknown = 0.13 where [OutsideDiameterItem] =  2.375;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A8" s="24">
+        <v>2.875</v>
+      </c>
+      <c r="B8" s="27">
+        <v>0.32724895833333334</v>
+      </c>
+      <c r="C8" s="27">
+        <v>0.49087343750000001</v>
+      </c>
+      <c r="D8" s="27">
+        <v>0.98174687500000002</v>
+      </c>
+      <c r="E8" s="27">
+        <v>0.32724895833333334</v>
+      </c>
+      <c r="F8" s="27">
+        <v>0.16362447916666667</v>
+      </c>
+      <c r="G8" s="27">
+        <v>0.24543671875</v>
+      </c>
+      <c r="H8" s="27">
+        <v>0.49087343750000001</v>
+      </c>
+      <c r="I8" s="27">
+        <v>0.16362447916666667</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V8" t="s">
+        <v>226</v>
+      </c>
+      <c r="W8" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  0.33, Degree90_1_5R =0.49, Degree90_3R = 0.98, Degree90_Unknown =0.33, Degree45_1R = 0.16, Degree45_1_5R =0.25, Degree45_3R = 0.49, Degree45_Unknown = 0.16 where [OutsideDiameterItem] =  2.875;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A9" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="B9" s="27">
+        <v>0.39269874999999993</v>
+      </c>
+      <c r="C9" s="27">
+        <v>0.58904812499999992</v>
+      </c>
+      <c r="D9" s="27">
+        <v>1.1780962499999998</v>
+      </c>
+      <c r="E9" s="27">
+        <v>0.39269874999999993</v>
+      </c>
+      <c r="F9" s="27">
+        <v>0.19634937499999996</v>
+      </c>
+      <c r="G9" s="27">
+        <v>0.29452406249999996</v>
+      </c>
+      <c r="H9" s="27">
+        <v>0.58904812499999992</v>
+      </c>
+      <c r="I9" s="27">
+        <v>0.19634937499999996</v>
+      </c>
+      <c r="J9" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V9" t="s">
+        <v>226</v>
+      </c>
+      <c r="W9" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  0.39, Degree90_1_5R =0.59, Degree90_3R = 1.18, Degree90_Unknown =0.39, Degree45_1R = 0.20, Degree45_1_5R =0.29, Degree45_3R = 0.59, Degree45_Unknown = 0.20 where [OutsideDiameterItem] =  3.5;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A10" s="24">
+        <v>4</v>
+      </c>
+      <c r="B10" s="27">
+        <v>0.45814854166666663</v>
+      </c>
+      <c r="C10" s="27">
+        <v>0.68722281249999995</v>
+      </c>
+      <c r="D10" s="27">
+        <v>1.3744456249999999</v>
+      </c>
+      <c r="E10" s="27">
+        <v>0.45814854166666663</v>
+      </c>
+      <c r="F10" s="27">
+        <v>0.22907427083333332</v>
+      </c>
+      <c r="G10" s="27">
+        <v>0.34361140624999997</v>
+      </c>
+      <c r="H10" s="27">
+        <v>0.68722281249999995</v>
+      </c>
+      <c r="I10" s="27">
+        <v>0.22907427083333332</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V10" t="s">
+        <v>226</v>
+      </c>
+      <c r="W10" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  0.46, Degree90_1_5R =0.69, Degree90_3R = 1.37, Degree90_Unknown =0.46, Degree45_1R = 0.23, Degree45_1_5R =0.34, Degree45_3R = 0.69, Degree45_Unknown = 0.23 where [OutsideDiameterItem] =  4;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A11" s="24">
+        <v>4.5</v>
+      </c>
+      <c r="B11" s="27">
+        <v>0.52359833333333328</v>
+      </c>
+      <c r="C11" s="27">
+        <v>0.78539749999999997</v>
+      </c>
+      <c r="D11" s="27">
+        <v>1.5707949999999999</v>
+      </c>
+      <c r="E11" s="27">
+        <v>0.52359833333333328</v>
+      </c>
+      <c r="F11" s="27">
+        <v>0.26179916666666664</v>
+      </c>
+      <c r="G11" s="27">
+        <v>0.39269874999999999</v>
+      </c>
+      <c r="H11" s="27">
+        <v>0.78539749999999997</v>
+      </c>
+      <c r="I11" s="27">
+        <v>0.26179916666666664</v>
+      </c>
+      <c r="J11" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V11" t="s">
+        <v>226</v>
+      </c>
+      <c r="W11" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  0.52, Degree90_1_5R =0.79, Degree90_3R = 1.57, Degree90_Unknown =0.52, Degree45_1R = 0.26, Degree45_1_5R =0.39, Degree45_3R = 0.79, Degree45_Unknown = 0.26 where [OutsideDiameterItem] =  4.5;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A12" s="24">
+        <v>5.5629999999999997</v>
+      </c>
+      <c r="B12" s="27">
+        <v>0.65449791666666668</v>
+      </c>
+      <c r="C12" s="27">
+        <v>0.98174687500000002</v>
+      </c>
+      <c r="D12" s="27">
+        <v>1.96349375</v>
+      </c>
+      <c r="E12" s="27">
+        <v>0.65449791666666668</v>
+      </c>
+      <c r="F12" s="27">
+        <v>0.32724895833333334</v>
+      </c>
+      <c r="G12" s="27">
+        <v>0.49087343750000001</v>
+      </c>
+      <c r="H12" s="27">
+        <v>0.98174687500000002</v>
+      </c>
+      <c r="I12" s="27">
+        <v>0.32724895833333334</v>
+      </c>
+      <c r="J12" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V12" t="s">
+        <v>226</v>
+      </c>
+      <c r="W12" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  0.65, Degree90_1_5R =0.98, Degree90_3R = 1.96, Degree90_Unknown =0.65, Degree45_1R = 0.33, Degree45_1_5R =0.49, Degree45_3R = 0.98, Degree45_Unknown = 0.33 where [OutsideDiameterItem] =  5.563;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A13" s="24">
+        <v>6.625</v>
+      </c>
+      <c r="B13" s="27">
+        <v>0.78539749999999986</v>
+      </c>
+      <c r="C13" s="27">
+        <v>1.1780962499999998</v>
+      </c>
+      <c r="D13" s="27">
+        <v>2.3561924999999997</v>
+      </c>
+      <c r="E13" s="27">
+        <v>0.78539749999999986</v>
+      </c>
+      <c r="F13" s="27">
+        <v>0.39269874999999993</v>
+      </c>
+      <c r="G13" s="27">
+        <v>0.58904812499999992</v>
+      </c>
+      <c r="H13" s="27">
+        <v>1.1780962499999998</v>
+      </c>
+      <c r="I13" s="27">
+        <v>0.39269874999999993</v>
+      </c>
+      <c r="J13" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V13" t="s">
+        <v>226</v>
+      </c>
+      <c r="W13" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  0.79, Degree90_1_5R =1.18, Degree90_3R = 2.36, Degree90_Unknown =0.79, Degree45_1R = 0.39, Degree45_1_5R =0.59, Degree45_3R = 1.18, Degree45_Unknown = 0.39 where [OutsideDiameterItem] =  6.625;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A14" s="24">
+        <v>8.625</v>
+      </c>
+      <c r="B14" s="27">
+        <v>1.0471966666666666</v>
+      </c>
+      <c r="C14" s="27">
+        <v>1.5707949999999999</v>
+      </c>
+      <c r="D14" s="27">
+        <v>3.1415899999999999</v>
+      </c>
+      <c r="E14" s="27">
+        <v>1.0471966666666666</v>
+      </c>
+      <c r="F14" s="27">
+        <v>0.52359833333333328</v>
+      </c>
+      <c r="G14" s="27">
+        <v>0.78539749999999997</v>
+      </c>
+      <c r="H14" s="27">
+        <v>1.5707949999999999</v>
+      </c>
+      <c r="I14" s="27">
+        <v>0.52359833333333328</v>
+      </c>
+      <c r="J14" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V14" t="s">
+        <v>226</v>
+      </c>
+      <c r="W14" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  1.05, Degree90_1_5R =1.57, Degree90_3R = 3.14, Degree90_Unknown =1.05, Degree45_1R = 0.52, Degree45_1_5R =0.79, Degree45_3R = 1.57, Degree45_Unknown = 0.52 where [OutsideDiameterItem] =  8.625;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A15" s="24">
+        <v>10.75</v>
+      </c>
+      <c r="B15" s="27">
+        <v>1.3089958333333334</v>
+      </c>
+      <c r="C15" s="27">
+        <v>1.96349375</v>
+      </c>
+      <c r="D15" s="27">
+        <v>3.9269875000000001</v>
+      </c>
+      <c r="E15" s="27">
+        <v>1.3089958333333334</v>
+      </c>
+      <c r="F15" s="27">
+        <v>0.65449791666666668</v>
+      </c>
+      <c r="G15" s="27">
+        <v>0.98174687500000002</v>
+      </c>
+      <c r="H15" s="27">
+        <v>1.96349375</v>
+      </c>
+      <c r="I15" s="27">
+        <v>0.65449791666666668</v>
+      </c>
+      <c r="J15" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V15" t="s">
+        <v>226</v>
+      </c>
+      <c r="W15" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  1.31, Degree90_1_5R =1.96, Degree90_3R = 3.93, Degree90_Unknown =1.31, Degree45_1R = 0.65, Degree45_1_5R =0.98, Degree45_3R = 1.96, Degree45_Unknown = 0.65 where [OutsideDiameterItem] =  10.75;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A16" s="24">
+        <v>12.75</v>
+      </c>
+      <c r="B16" s="27">
+        <v>1.5707949999999997</v>
+      </c>
+      <c r="C16" s="27">
+        <v>2.3561924999999997</v>
+      </c>
+      <c r="D16" s="27">
+        <v>4.7123849999999994</v>
+      </c>
+      <c r="E16" s="27">
+        <v>1.5707949999999997</v>
+      </c>
+      <c r="F16" s="27">
+        <v>0.78539749999999986</v>
+      </c>
+      <c r="G16" s="27">
+        <v>1.1780962499999998</v>
+      </c>
+      <c r="H16" s="27">
+        <v>2.3561924999999997</v>
+      </c>
+      <c r="I16" s="27">
+        <v>0.78539749999999986</v>
+      </c>
+      <c r="J16" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V16" t="s">
+        <v>226</v>
+      </c>
+      <c r="W16" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  1.57, Degree90_1_5R =2.36, Degree90_3R = 4.71, Degree90_Unknown =1.57, Degree45_1R = 0.79, Degree45_1_5R =1.18, Degree45_3R = 2.36, Degree45_Unknown = 0.79 where [OutsideDiameterItem] =  12.75;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A17" s="24">
+        <v>14</v>
+      </c>
+      <c r="B17" s="27">
+        <v>1.8325941666666665</v>
+      </c>
+      <c r="C17" s="27">
+        <v>2.7488912499999998</v>
+      </c>
+      <c r="D17" s="27">
+        <v>5.4977824999999996</v>
+      </c>
+      <c r="E17" s="27">
+        <v>1.8325941666666665</v>
+      </c>
+      <c r="F17" s="27">
+        <v>0.91629708333333326</v>
+      </c>
+      <c r="G17" s="27">
+        <v>1.3744456249999999</v>
+      </c>
+      <c r="H17" s="27">
+        <v>2.7488912499999998</v>
+      </c>
+      <c r="I17" s="27">
+        <v>0.91629708333333326</v>
+      </c>
+      <c r="J17" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S17" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V17" t="s">
+        <v>226</v>
+      </c>
+      <c r="W17" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  1.83, Degree90_1_5R =2.75, Degree90_3R = 5.50, Degree90_Unknown =1.83, Degree45_1R = 0.92, Degree45_1_5R =1.37, Degree45_3R = 2.75, Degree45_Unknown = 0.92 where [OutsideDiameterItem] =  14;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A18" s="24">
+        <v>16</v>
+      </c>
+      <c r="B18" s="27">
+        <v>2.0943933333333331</v>
+      </c>
+      <c r="C18" s="27">
+        <v>3.1415899999999999</v>
+      </c>
+      <c r="D18" s="27">
+        <v>6.2831799999999998</v>
+      </c>
+      <c r="E18" s="27">
+        <v>2.0943933333333331</v>
+      </c>
+      <c r="F18" s="27">
+        <v>1.0471966666666666</v>
+      </c>
+      <c r="G18" s="27">
+        <v>1.5707949999999999</v>
+      </c>
+      <c r="H18" s="27">
+        <v>3.1415899999999999</v>
+      </c>
+      <c r="I18" s="27">
+        <v>1.0471966666666666</v>
+      </c>
+      <c r="J18" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T18" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V18" t="s">
+        <v>226</v>
+      </c>
+      <c r="W18" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  2.09, Degree90_1_5R =3.14, Degree90_3R = 6.28, Degree90_Unknown =2.09, Degree45_1R = 1.05, Degree45_1_5R =1.57, Degree45_3R = 3.14, Degree45_Unknown = 1.05 where [OutsideDiameterItem] =  16;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A19" s="24">
+        <v>18</v>
+      </c>
+      <c r="B19" s="27">
+        <v>2.3561925000000001</v>
+      </c>
+      <c r="C19" s="27">
+        <v>3.53428875</v>
+      </c>
+      <c r="D19" s="27">
+        <v>7.0685775</v>
+      </c>
+      <c r="E19" s="27">
+        <v>2.3561925000000001</v>
+      </c>
+      <c r="F19" s="27">
+        <v>1.1780962500000001</v>
+      </c>
+      <c r="G19" s="27">
+        <v>1.767144375</v>
+      </c>
+      <c r="H19" s="27">
+        <v>3.53428875</v>
+      </c>
+      <c r="I19" s="27">
+        <v>1.1780962500000001</v>
+      </c>
+      <c r="J19" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T19" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V19" t="s">
+        <v>226</v>
+      </c>
+      <c r="W19" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  2.36, Degree90_1_5R =3.53, Degree90_3R = 7.07, Degree90_Unknown =2.36, Degree45_1R = 1.18, Degree45_1_5R =1.77, Degree45_3R = 3.53, Degree45_Unknown = 1.18 where [OutsideDiameterItem] =  18;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A20" s="24">
+        <v>20</v>
+      </c>
+      <c r="B20" s="27">
+        <v>2.6179916666666667</v>
+      </c>
+      <c r="C20" s="27">
+        <v>3.9269875000000001</v>
+      </c>
+      <c r="D20" s="27">
+        <v>7.8539750000000002</v>
+      </c>
+      <c r="E20" s="27">
+        <v>2.6179916666666667</v>
+      </c>
+      <c r="F20" s="27">
+        <v>1.3089958333333334</v>
+      </c>
+      <c r="G20" s="27">
+        <v>1.96349375</v>
+      </c>
+      <c r="H20" s="27">
+        <v>3.9269875000000001</v>
+      </c>
+      <c r="I20" s="27">
+        <v>1.3089958333333334</v>
+      </c>
+      <c r="J20" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T20" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V20" t="s">
+        <v>226</v>
+      </c>
+      <c r="W20" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  2.62, Degree90_1_5R =3.93, Degree90_3R = 7.85, Degree90_Unknown =2.62, Degree45_1R = 1.31, Degree45_1_5R =1.96, Degree45_3R = 3.93, Degree45_Unknown = 1.31 where [OutsideDiameterItem] =  20;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A21" s="24">
+        <v>22</v>
+      </c>
+      <c r="B21" s="27">
+        <v>2.8797908333333333</v>
+      </c>
+      <c r="C21" s="27">
+        <v>4.3196862500000002</v>
+      </c>
+      <c r="D21" s="27">
+        <v>8.6393725000000003</v>
+      </c>
+      <c r="E21" s="27">
+        <v>2.8797908333333333</v>
+      </c>
+      <c r="F21" s="27">
+        <v>1.4398954166666666</v>
+      </c>
+      <c r="G21" s="27">
+        <v>2.1598431250000001</v>
+      </c>
+      <c r="H21" s="27">
+        <v>4.3196862500000002</v>
+      </c>
+      <c r="I21" s="27">
+        <v>1.4398954166666666</v>
+      </c>
+      <c r="J21" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T21" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V21" t="s">
+        <v>226</v>
+      </c>
+      <c r="W21" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  2.88, Degree90_1_5R =4.32, Degree90_3R = 8.64, Degree90_Unknown =2.88, Degree45_1R = 1.44, Degree45_1_5R =2.16, Degree45_3R = 4.32, Degree45_Unknown = 1.44 where [OutsideDiameterItem] =  22;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A22" s="24">
+        <v>24</v>
+      </c>
+      <c r="B22" s="27">
+        <v>3.1415899999999994</v>
+      </c>
+      <c r="C22" s="27">
+        <v>4.7123849999999994</v>
+      </c>
+      <c r="D22" s="27">
+        <v>9.4247699999999988</v>
+      </c>
+      <c r="E22" s="27">
+        <v>3.1415899999999994</v>
+      </c>
+      <c r="F22" s="27">
+        <v>1.5707949999999997</v>
+      </c>
+      <c r="G22" s="27">
+        <v>2.3561924999999997</v>
+      </c>
+      <c r="H22" s="27">
+        <v>4.7123849999999994</v>
+      </c>
+      <c r="I22" s="27">
+        <v>1.5707949999999997</v>
+      </c>
+      <c r="J22" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S22" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T22" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V22" t="s">
+        <v>226</v>
+      </c>
+      <c r="W22" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  3.14, Degree90_1_5R =4.71, Degree90_3R = 9.42, Degree90_Unknown =3.14, Degree45_1R = 1.57, Degree45_1_5R =2.36, Degree45_3R = 4.71, Degree45_Unknown = 1.57 where [OutsideDiameterItem] =  24;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A23" s="24">
+        <v>26</v>
+      </c>
+      <c r="B23" s="27">
+        <v>3.4033891666666665</v>
+      </c>
+      <c r="C23" s="27">
+        <v>5.1050837499999995</v>
+      </c>
+      <c r="D23" s="27">
+        <v>10.210167499999999</v>
+      </c>
+      <c r="E23" s="27">
+        <v>3.4033891666666665</v>
+      </c>
+      <c r="F23" s="27">
+        <v>1.7016945833333332</v>
+      </c>
+      <c r="G23" s="27">
+        <v>2.5525418749999997</v>
+      </c>
+      <c r="H23" s="27">
+        <v>5.1050837499999995</v>
+      </c>
+      <c r="I23" s="27">
+        <v>1.7016945833333332</v>
+      </c>
+      <c r="J23" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R23" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S23" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T23" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V23" t="s">
+        <v>226</v>
+      </c>
+      <c r="W23" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  3.40, Degree90_1_5R =5.11, Degree90_3R = 10.21, Degree90_Unknown =3.40, Degree45_1R = 1.70, Degree45_1_5R =2.55, Degree45_3R = 5.11, Degree45_Unknown = 1.70 where [OutsideDiameterItem] =  26;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A24" s="24">
+        <v>30</v>
+      </c>
+      <c r="B24" s="27">
+        <v>3.9269874999999996</v>
+      </c>
+      <c r="C24" s="27">
+        <v>5.8904812499999997</v>
+      </c>
+      <c r="D24" s="27">
+        <v>11.780962499999999</v>
+      </c>
+      <c r="E24" s="27">
+        <v>3.9269874999999996</v>
+      </c>
+      <c r="F24" s="27">
+        <v>1.9634937499999998</v>
+      </c>
+      <c r="G24" s="27">
+        <v>2.9452406249999998</v>
+      </c>
+      <c r="H24" s="27">
+        <v>5.8904812499999997</v>
+      </c>
+      <c r="I24" s="27">
+        <v>1.9634937499999998</v>
+      </c>
+      <c r="J24" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P24" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q24" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R24" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S24" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T24" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V24" t="s">
+        <v>226</v>
+      </c>
+      <c r="W24" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  3.93, Degree90_1_5R =5.89, Degree90_3R = 11.78, Degree90_Unknown =3.93, Degree45_1R = 1.96, Degree45_1_5R =2.95, Degree45_3R = 5.89, Degree45_Unknown = 1.96 where [OutsideDiameterItem] =  30;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A25" s="24">
+        <v>34</v>
+      </c>
+      <c r="B25" s="27">
+        <v>4.4505858333333332</v>
+      </c>
+      <c r="C25" s="27">
+        <v>6.6758787499999999</v>
+      </c>
+      <c r="D25" s="27">
+        <v>13.3517575</v>
+      </c>
+      <c r="E25" s="27">
+        <v>4.4505858333333332</v>
+      </c>
+      <c r="F25" s="27">
+        <v>2.2252929166666666</v>
+      </c>
+      <c r="G25" s="27">
+        <v>3.3379393749999999</v>
+      </c>
+      <c r="H25" s="27">
+        <v>6.6758787499999999</v>
+      </c>
+      <c r="I25" s="27">
+        <v>2.2252929166666666</v>
+      </c>
+      <c r="J25" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P25" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q25" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R25" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S25" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T25" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V25" t="s">
+        <v>226</v>
+      </c>
+      <c r="W25" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  4.45, Degree90_1_5R =6.68, Degree90_3R = 13.35, Degree90_Unknown =4.45, Degree45_1R = 2.23, Degree45_1_5R =3.34, Degree45_3R = 6.68, Degree45_Unknown = 2.23 where [OutsideDiameterItem] =  34;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A26" s="24">
+        <v>36</v>
+      </c>
+      <c r="B26" s="27">
+        <v>4.7123850000000003</v>
+      </c>
+      <c r="C26" s="27">
+        <v>7.0685775</v>
+      </c>
+      <c r="D26" s="27">
+        <v>14.137155</v>
+      </c>
+      <c r="E26" s="27">
+        <v>4.7123850000000003</v>
+      </c>
+      <c r="F26" s="27">
+        <v>2.3561925000000001</v>
+      </c>
+      <c r="G26" s="27">
+        <v>3.53428875</v>
+      </c>
+      <c r="H26" s="27">
+        <v>7.0685775</v>
+      </c>
+      <c r="I26" s="27">
+        <v>2.3561925000000001</v>
+      </c>
+      <c r="J26" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P26" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q26" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R26" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S26" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T26" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V26" t="s">
+        <v>226</v>
+      </c>
+      <c r="W26" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  4.71, Degree90_1_5R =7.07, Degree90_3R = 14.14, Degree90_Unknown =4.71, Degree45_1R = 2.36, Degree45_1_5R =3.53, Degree45_3R = 7.07, Degree45_Unknown = 2.36 where [OutsideDiameterItem] =  36;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A27" s="24">
+        <v>42</v>
+      </c>
+      <c r="B27" s="27">
+        <v>5.4977824999999996</v>
+      </c>
+      <c r="C27" s="27">
+        <v>8.2466737499999994</v>
+      </c>
+      <c r="D27" s="27">
+        <v>16.493347499999999</v>
+      </c>
+      <c r="E27" s="27">
+        <v>5.4977824999999996</v>
+      </c>
+      <c r="F27" s="27">
+        <v>2.7488912499999998</v>
+      </c>
+      <c r="G27" s="27">
+        <v>4.1233368749999997</v>
+      </c>
+      <c r="H27" s="27">
+        <v>8.2466737499999994</v>
+      </c>
+      <c r="I27" s="27">
+        <v>2.7488912499999998</v>
+      </c>
+      <c r="J27" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N27" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O27" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P27" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q27" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="R27" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="S27" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="T27" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="V27" t="s">
+        <v>226</v>
+      </c>
+      <c r="W27" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE [dbo].[OutsideDiameters] set Degree90_1R =  5.50, Degree90_1_5R =8.25, Degree90_3R = 16.49, Degree90_Unknown =5.50, Degree45_1R = 2.75, Degree45_1_5R =4.12, Degree45_3R = 8.25, Degree45_Unknown = 2.75 where [OutsideDiameterItem] =  42;</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4ADC09-6FC6-4AEB-9166-C40875F8B380}">
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="15.41015625" customWidth="1"/>
+    <col min="2" max="2" width="26.64453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A1" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A2" s="24">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="B2" s="25">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A3" s="24">
+        <v>0.54</v>
+      </c>
+      <c r="B3" s="25">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A4" s="24">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="B4" s="25">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A5" s="24">
+        <v>0.84</v>
+      </c>
+      <c r="B5" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A6" s="24">
+        <v>1.05</v>
+      </c>
+      <c r="B6" s="25">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A7" s="24">
+        <v>1.3149999999999999</v>
+      </c>
+      <c r="B7" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A8" s="24">
+        <v>1.66</v>
+      </c>
+      <c r="B8" s="25">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A9" s="24">
+        <v>1.9</v>
+      </c>
+      <c r="B9" s="25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A10" s="24">
+        <v>2.375</v>
+      </c>
+      <c r="B10" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A11" s="24">
+        <v>2.875</v>
+      </c>
+      <c r="B11" s="25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A12" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="B12" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A13" s="24">
+        <v>4</v>
+      </c>
+      <c r="B13" s="25">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A14" s="24">
+        <v>4.5</v>
+      </c>
+      <c r="B14" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A15" s="24">
+        <v>5.5629999999999997</v>
+      </c>
+      <c r="B15" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A16" s="24">
+        <v>6.625</v>
+      </c>
+      <c r="B16" s="25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A17" s="24">
+        <v>8.625</v>
+      </c>
+      <c r="B17" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A18" s="24">
+        <v>10.75</v>
+      </c>
+      <c r="B18" s="25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A19" s="24">
+        <v>12.75</v>
+      </c>
+      <c r="B19" s="25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A20" s="24">
+        <v>14</v>
+      </c>
+      <c r="B20" s="25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A21" s="24">
+        <v>16</v>
+      </c>
+      <c r="B21" s="25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A22" s="24">
+        <v>18</v>
+      </c>
+      <c r="B22" s="25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A23" s="24">
+        <v>20</v>
+      </c>
+      <c r="B23" s="25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A24" s="24">
+        <v>22</v>
+      </c>
+      <c r="B24" s="25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A25" s="24">
+        <v>24</v>
+      </c>
+      <c r="B25" s="25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A26" s="24">
+        <v>26</v>
+      </c>
+      <c r="B26" s="25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A27" s="24">
+        <v>28</v>
+      </c>
+      <c r="B27" s="25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A28" s="24">
+        <v>30</v>
+      </c>
+      <c r="B28" s="25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A29" s="24">
+        <v>32</v>
+      </c>
+      <c r="B29" s="25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A30" s="24">
+        <v>34</v>
+      </c>
+      <c r="B30" s="25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A31" s="24">
+        <v>36</v>
+      </c>
+      <c r="B31" s="25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A32" s="24">
+        <v>42</v>
+      </c>
+      <c r="B32" s="25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9588CA03-9F97-4B44-A094-0D155E362BAD}">
   <dimension ref="A1:G73"/>
   <sheetViews>
@@ -3247,7 +5643,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE5411D-180F-4784-9130-29A4097D29B2}">
   <dimension ref="A1:F28"/>
   <sheetViews>
@@ -3257,23 +5653,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="6" max="6" width="11.703125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="11.703125" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" t="s">
         <v>122</v>
       </c>
-      <c r="B1" t="s">
-        <v>123</v>
-      </c>
       <c r="D1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" t="s">
         <v>149</v>
       </c>
-      <c r="E1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="11" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3282,15 +5678,15 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F2" s="15">
+        <v>123</v>
+      </c>
+      <c r="F2" s="11">
         <v>25000</v>
       </c>
     </row>
@@ -3299,15 +5695,15 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F3" s="15">
+        <v>124</v>
+      </c>
+      <c r="F3" s="11">
         <v>30000</v>
       </c>
     </row>
@@ -3316,15 +5712,15 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>126</v>
-      </c>
-      <c r="F4" s="15">
+        <v>125</v>
+      </c>
+      <c r="F4" s="11">
         <v>35000</v>
       </c>
     </row>
@@ -3333,15 +5729,15 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F5" s="15">
+        <v>126</v>
+      </c>
+      <c r="F5" s="11">
         <v>35000</v>
       </c>
     </row>
@@ -3350,15 +5746,15 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>128</v>
-      </c>
-      <c r="F6" s="15">
+        <v>127</v>
+      </c>
+      <c r="F6" s="11">
         <v>30000</v>
       </c>
     </row>
@@ -3367,15 +5763,15 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F7" s="15">
+        <v>128</v>
+      </c>
+      <c r="F7" s="11">
         <v>35000</v>
       </c>
     </row>
@@ -3384,15 +5780,15 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>130</v>
-      </c>
-      <c r="F8" s="15">
+        <v>129</v>
+      </c>
+      <c r="F8" s="11">
         <v>40000</v>
       </c>
     </row>
@@ -3401,15 +5797,15 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>131</v>
-      </c>
-      <c r="F9" s="15">
+        <v>130</v>
+      </c>
+      <c r="F9" s="11">
         <v>35000</v>
       </c>
     </row>
@@ -3418,15 +5814,15 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D10">
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F10" s="15">
+        <v>131</v>
+      </c>
+      <c r="F10" s="11">
         <v>40000</v>
       </c>
     </row>
@@ -3435,15 +5831,15 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D11">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F11" s="15">
+        <v>132</v>
+      </c>
+      <c r="F11" s="11">
         <v>35000</v>
       </c>
     </row>
@@ -3452,15 +5848,15 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D12">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>134</v>
-      </c>
-      <c r="F12" s="15">
+        <v>133</v>
+      </c>
+      <c r="F12" s="11">
         <v>46000</v>
       </c>
     </row>
@@ -3469,15 +5865,15 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D13">
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>135</v>
-      </c>
-      <c r="F13" s="15">
+        <v>134</v>
+      </c>
+      <c r="F13" s="11">
         <v>42000</v>
       </c>
     </row>
@@ -3486,15 +5882,15 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D14">
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>136</v>
-      </c>
-      <c r="F14" s="15">
+        <v>135</v>
+      </c>
+      <c r="F14" s="11">
         <v>46000</v>
       </c>
     </row>
@@ -3503,15 +5899,15 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D15">
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>137</v>
-      </c>
-      <c r="F15" s="15">
+        <v>136</v>
+      </c>
+      <c r="F15" s="11">
         <v>48000</v>
       </c>
     </row>
@@ -3520,15 +5916,15 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D16">
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>138</v>
-      </c>
-      <c r="F16" s="15">
+        <v>137</v>
+      </c>
+      <c r="F16" s="11">
         <v>52000</v>
       </c>
     </row>
@@ -3537,15 +5933,15 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D17">
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>139</v>
-      </c>
-      <c r="F17" s="15">
+        <v>138</v>
+      </c>
+      <c r="F17" s="11">
         <v>60000</v>
       </c>
     </row>
@@ -3554,15 +5950,15 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D18">
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>140</v>
-      </c>
-      <c r="F18" s="15">
+        <v>139</v>
+      </c>
+      <c r="F18" s="11">
         <v>65000</v>
       </c>
     </row>
@@ -3571,15 +5967,15 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D19">
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>141</v>
-      </c>
-      <c r="F19" s="15">
+        <v>140</v>
+      </c>
+      <c r="F19" s="11">
         <v>70000</v>
       </c>
     </row>
@@ -3588,15 +5984,15 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D20">
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>142</v>
-      </c>
-      <c r="F20" s="15">
+        <v>141</v>
+      </c>
+      <c r="F20" s="11">
         <v>42000</v>
       </c>
     </row>
@@ -3605,15 +6001,15 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D21">
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>143</v>
-      </c>
-      <c r="F21" s="15">
+        <v>142</v>
+      </c>
+      <c r="F21" s="11">
         <v>46000</v>
       </c>
     </row>
@@ -3622,15 +6018,15 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D22">
         <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>144</v>
-      </c>
-      <c r="F22" s="15">
+        <v>143</v>
+      </c>
+      <c r="F22" s="11">
         <v>48000</v>
       </c>
     </row>
@@ -3639,15 +6035,15 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D23">
         <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>145</v>
-      </c>
-      <c r="F23" s="15">
+        <v>144</v>
+      </c>
+      <c r="F23" s="11">
         <v>52000</v>
       </c>
     </row>
@@ -3656,15 +6052,15 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D24">
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>146</v>
-      </c>
-      <c r="F24" s="15">
+        <v>145</v>
+      </c>
+      <c r="F24" s="11">
         <v>60000</v>
       </c>
     </row>
@@ -3673,15 +6069,15 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D25">
         <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>147</v>
-      </c>
-      <c r="F25" s="15">
+        <v>146</v>
+      </c>
+      <c r="F25" s="11">
         <v>65000</v>
       </c>
     </row>
@@ -3690,15 +6086,15 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D26">
         <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>148</v>
-      </c>
-      <c r="F26" s="15">
+        <v>147</v>
+      </c>
+      <c r="F26" s="11">
         <v>70000</v>
       </c>
     </row>
@@ -3715,7 +6111,7 @@
       <c r="E27" t="s">
         <v>91</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="11">
         <v>24000</v>
       </c>
     </row>
@@ -3732,7 +6128,7 @@
       <c r="E28" t="s">
         <v>92</v>
       </c>
-      <c r="F28" s="15">
+      <c r="F28" s="11">
         <v>24000</v>
       </c>
     </row>
@@ -3742,7 +6138,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA8AC4CB-2FBB-4210-B98D-A77C046C80A0}">
   <dimension ref="A1:G16"/>
   <sheetViews>
@@ -3756,28 +6152,28 @@
     <col min="2" max="2" width="24.8203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.46875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.8203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5859375" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5859375" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" t="s">
         <v>151</v>
       </c>
-      <c r="B1" t="s">
-        <v>152</v>
-      </c>
       <c r="D1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" t="s">
         <v>167</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" t="s">
         <v>169</v>
-      </c>
-      <c r="G1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.5">
@@ -3785,15 +6181,15 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F2" s="15">
+        <v>152</v>
+      </c>
+      <c r="F2" s="11">
         <v>0.6</v>
       </c>
     </row>
@@ -3802,15 +6198,15 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>154</v>
-      </c>
-      <c r="F3" s="15">
+        <v>153</v>
+      </c>
+      <c r="F3" s="11">
         <v>1</v>
       </c>
     </row>
@@ -3819,15 +6215,15 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
-      </c>
-      <c r="F4" s="15">
+        <v>154</v>
+      </c>
+      <c r="F4" s="11">
         <v>1</v>
       </c>
     </row>
@@ -3836,15 +6232,15 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F5" s="15">
+        <v>155</v>
+      </c>
+      <c r="F5" s="11">
         <v>1</v>
       </c>
     </row>
@@ -3853,15 +6249,15 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>157</v>
-      </c>
-      <c r="F6" s="15">
+        <v>156</v>
+      </c>
+      <c r="F6" s="11">
         <v>1</v>
       </c>
     </row>
@@ -3870,15 +6266,15 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>158</v>
-      </c>
-      <c r="F7" s="15">
+        <v>157</v>
+      </c>
+      <c r="F7" s="11">
         <v>1</v>
       </c>
     </row>
@@ -3887,15 +6283,15 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>159</v>
-      </c>
-      <c r="F8" s="15">
+        <v>158</v>
+      </c>
+      <c r="F8" s="11">
         <v>1</v>
       </c>
     </row>
@@ -3904,15 +6300,15 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F9" s="15">
+        <v>170</v>
+      </c>
+      <c r="F9" s="11">
         <v>1</v>
       </c>
     </row>
@@ -3921,15 +6317,15 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D10">
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>161</v>
-      </c>
-      <c r="F10" s="15">
+        <v>160</v>
+      </c>
+      <c r="F10" s="11">
         <v>1</v>
       </c>
     </row>
@@ -3938,15 +6334,15 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D11">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>162</v>
-      </c>
-      <c r="F11" s="15">
+        <v>161</v>
+      </c>
+      <c r="F11" s="11">
         <v>1</v>
       </c>
     </row>
@@ -3955,15 +6351,15 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D12">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>163</v>
-      </c>
-      <c r="F12" s="15">
+        <v>162</v>
+      </c>
+      <c r="F12" s="11">
         <v>0.8</v>
       </c>
     </row>
@@ -3972,15 +6368,15 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D13">
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>164</v>
-      </c>
-      <c r="F13" s="15">
+        <v>163</v>
+      </c>
+      <c r="F13" s="11">
         <v>0.6</v>
       </c>
     </row>
@@ -3989,15 +6385,15 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D14">
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>165</v>
-      </c>
-      <c r="F14" s="15">
+        <v>164</v>
+      </c>
+      <c r="F14" s="11">
         <v>1</v>
       </c>
     </row>
@@ -4006,15 +6402,15 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D15">
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>166</v>
-      </c>
-      <c r="F15" s="15">
+        <v>165</v>
+      </c>
+      <c r="F15" s="11">
         <v>1</v>
       </c>
     </row>
@@ -4031,11 +6427,11 @@
       <c r="E16" t="s">
         <v>91</v>
       </c>
-      <c r="F16" s="15" t="s">
-        <v>172</v>
+      <c r="F16" s="11" t="s">
+        <v>171</v>
       </c>
       <c r="G16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>